<commit_message>
made facebook videos page
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0117F104-C524-4FDF-81C6-706631AD9882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075EEFD6-BBDD-4534-B478-26A26304868A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="347">
   <si>
     <t>shopify_orders</t>
   </si>
@@ -1017,6 +1017,51 @@
   </si>
   <si>
     <t>organicGoogleSearchImpressions</t>
+  </si>
+  <si>
+    <t>facebook_videos</t>
+  </si>
+  <si>
+    <t>post_video_likes_by_reaction_type</t>
+  </si>
+  <si>
+    <t>post_video_avg_time_watched</t>
+  </si>
+  <si>
+    <t>post_video_social_actions</t>
+  </si>
+  <si>
+    <t>post_video_view_time</t>
+  </si>
+  <si>
+    <t>post_impressions_unique</t>
+  </si>
+  <si>
+    <t>blue_reels_play_count</t>
+  </si>
+  <si>
+    <t>fb_reels_total_plays</t>
+  </si>
+  <si>
+    <t>fb_reels_replay_count</t>
+  </si>
+  <si>
+    <t>post_video_retention_graph</t>
+  </si>
+  <si>
+    <t>post_video_followers</t>
+  </si>
+  <si>
+    <t>post_video_likes_by_reaction_type.REACTION_LIKE</t>
+  </si>
+  <si>
+    <t>post_video_likes_by_reaction_type.REACTION_LOVE</t>
+  </si>
+  <si>
+    <t>post_video_social_actions.COMMENT</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
@@ -1874,10 +1919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ17"/>
+  <dimension ref="A1:BJ18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BG3" sqref="BG3"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2664,55 +2709,55 @@
       <c r="AR5" t="s">
         <v>92</v>
       </c>
-      <c r="AS5" s="3" t="s">
+      <c r="AS5" t="s">
         <v>303</v>
       </c>
-      <c r="AT5" s="3" t="s">
+      <c r="AT5" t="s">
         <v>304</v>
       </c>
-      <c r="AU5" s="3" t="s">
+      <c r="AU5" t="s">
         <v>305</v>
       </c>
-      <c r="AV5" s="3" t="s">
+      <c r="AV5" t="s">
         <v>306</v>
       </c>
-      <c r="AW5" s="3" t="s">
+      <c r="AW5" t="s">
         <v>307</v>
       </c>
-      <c r="AX5" s="3" t="s">
+      <c r="AX5" t="s">
         <v>308</v>
       </c>
-      <c r="AY5" s="3" t="s">
+      <c r="AY5" t="s">
         <v>309</v>
       </c>
-      <c r="AZ5" s="3" t="s">
+      <c r="AZ5" t="s">
         <v>310</v>
       </c>
-      <c r="BA5" s="3" t="s">
+      <c r="BA5" t="s">
         <v>50</v>
       </c>
-      <c r="BB5" s="3" t="s">
+      <c r="BB5" t="s">
         <v>69</v>
       </c>
-      <c r="BC5" s="3" t="s">
+      <c r="BC5" t="s">
         <v>311</v>
       </c>
-      <c r="BD5" s="3" t="s">
+      <c r="BD5" t="s">
         <v>312</v>
       </c>
-      <c r="BE5" s="3" t="s">
+      <c r="BE5" t="s">
         <v>67</v>
       </c>
-      <c r="BF5" s="3" t="s">
+      <c r="BF5" t="s">
         <v>308</v>
       </c>
-      <c r="BG5" s="3" t="s">
+      <c r="BG5" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>93</v>
+        <v>332</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>94</v>
@@ -2721,311 +2766,365 @@
         <v>314</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>346</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>343</v>
       </c>
       <c r="F6" t="s">
-        <v>97</v>
+        <v>344</v>
       </c>
       <c r="G6" t="s">
-        <v>98</v>
+        <v>345</v>
       </c>
       <c r="H6" t="s">
-        <v>99</v>
+        <v>333</v>
       </c>
       <c r="I6" t="s">
-        <v>100</v>
+        <v>334</v>
       </c>
       <c r="J6" t="s">
-        <v>101</v>
+        <v>335</v>
       </c>
       <c r="K6" t="s">
-        <v>102</v>
+        <v>336</v>
       </c>
       <c r="L6" t="s">
-        <v>103</v>
+        <v>337</v>
       </c>
       <c r="M6" t="s">
-        <v>104</v>
+        <v>338</v>
+      </c>
+      <c r="N6" t="s">
+        <v>339</v>
+      </c>
+      <c r="O6" t="s">
+        <v>340</v>
+      </c>
+      <c r="P6" t="s">
+        <v>341</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" t="s">
-        <v>89</v>
+        <v>93</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>314</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>96</v>
+      </c>
+      <c r="F7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H7" t="s">
+        <v>99</v>
+      </c>
+      <c r="I7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J7" t="s">
+        <v>101</v>
+      </c>
+      <c r="K7" t="s">
+        <v>102</v>
+      </c>
+      <c r="L7" t="s">
+        <v>103</v>
+      </c>
+      <c r="M7" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="E8" t="s">
-        <v>110</v>
-      </c>
-      <c r="F8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G8" t="s">
-        <v>112</v>
-      </c>
-      <c r="H8" t="s">
-        <v>113</v>
-      </c>
-      <c r="I8" t="s">
-        <v>114</v>
-      </c>
-      <c r="J8" t="s">
-        <v>115</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="V8" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="W8" s="3" t="s">
-        <v>327</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>106</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" t="s">
+        <v>108</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E9" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F9" t="s">
-        <v>97</v>
+        <v>111</v>
+      </c>
+      <c r="G9" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I9" t="s">
+        <v>114</v>
+      </c>
+      <c r="J9" t="s">
+        <v>115</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C10" t="s">
-        <v>122</v>
+        <v>116</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E10" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F10" t="s">
-        <v>125</v>
-      </c>
-      <c r="G10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H10" t="s">
-        <v>127</v>
-      </c>
-      <c r="I10" t="s">
-        <v>128</v>
-      </c>
-      <c r="J10" t="s">
-        <v>129</v>
-      </c>
-      <c r="K10" t="s">
-        <v>130</v>
-      </c>
-      <c r="L10" t="s">
-        <v>131</v>
-      </c>
-      <c r="M10" t="s">
-        <v>132</v>
-      </c>
-      <c r="N10" t="s">
-        <v>133</v>
-      </c>
-      <c r="O10" t="s">
-        <v>134</v>
-      </c>
-      <c r="P10" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>136</v>
-      </c>
-      <c r="R10" t="s">
-        <v>137</v>
-      </c>
-      <c r="S10" t="s">
-        <v>138</v>
-      </c>
-      <c r="T10" t="s">
-        <v>139</v>
-      </c>
-      <c r="U10" t="s">
-        <v>140</v>
-      </c>
-      <c r="V10" t="s">
-        <v>141</v>
-      </c>
-      <c r="W10" t="s">
-        <v>142</v>
-      </c>
-      <c r="X10" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z10" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="AA10" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="AB10" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="AC10" s="3" t="s">
-        <v>331</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H11" t="s">
+        <v>127</v>
+      </c>
+      <c r="I11" t="s">
+        <v>128</v>
+      </c>
+      <c r="J11" t="s">
+        <v>129</v>
+      </c>
+      <c r="K11" t="s">
+        <v>130</v>
+      </c>
+      <c r="L11" t="s">
+        <v>131</v>
+      </c>
+      <c r="M11" t="s">
+        <v>132</v>
+      </c>
+      <c r="N11" t="s">
+        <v>133</v>
+      </c>
+      <c r="O11" t="s">
+        <v>134</v>
+      </c>
+      <c r="P11" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>136</v>
+      </c>
+      <c r="R11" t="s">
+        <v>137</v>
+      </c>
+      <c r="S11" t="s">
+        <v>138</v>
+      </c>
+      <c r="T11" t="s">
+        <v>139</v>
+      </c>
+      <c r="U11" t="s">
+        <v>140</v>
+      </c>
+      <c r="V11" t="s">
+        <v>141</v>
+      </c>
+      <c r="W11" t="s">
+        <v>142</v>
+      </c>
+      <c r="X11" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z11" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>146</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>147</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>148</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>149</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>150</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>151</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H12" t="s">
         <v>152</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I12" t="s">
         <v>153</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J12" t="s">
         <v>154</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K12" t="s">
         <v>155</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L12" t="s">
         <v>156</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M12" t="s">
         <v>157</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N12" t="s">
         <v>158</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O12" t="s">
         <v>159</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P12" t="s">
         <v>160</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q12" t="s">
         <v>161</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R12" t="s">
         <v>162</v>
       </c>
-      <c r="S11" t="s">
+      <c r="S12" t="s">
         <v>163</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T12" t="s">
         <v>164</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U12" t="s">
         <v>165</v>
       </c>
-      <c r="V11" t="s">
+      <c r="V12" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>169</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
more cleanup for weekly report 5
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075EEFD6-BBDD-4534-B478-26A26304868A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C20FDE-B97C-4E86-B3D1-1E4CC24E3DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1921,8 +1921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2375,7 +2375,7 @@
       <c r="AI3" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AJ3" s="3" t="s">
         <v>33</v>
       </c>
       <c r="AK3" s="3" t="s">
@@ -2667,19 +2667,19 @@
       <c r="AD5" t="s">
         <v>78</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AE5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AF5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AG5" s="3" t="s">
         <v>81</v>
       </c>
       <c r="AH5" t="s">
         <v>82</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AI5" s="3" t="s">
         <v>83</v>
       </c>
       <c r="AJ5" t="s">
@@ -2985,25 +2985,25 @@
       <c r="I11" t="s">
         <v>128</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="3" t="s">
         <v>131</v>
       </c>
       <c r="M11" t="s">
         <v>132</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="3" t="s">
         <v>133</v>
       </c>
       <c r="O11" t="s">
         <v>134</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="3" t="s">
         <v>135</v>
       </c>
       <c r="Q11" t="s">
@@ -3015,22 +3015,22 @@
       <c r="S11" t="s">
         <v>138</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11" s="3" t="s">
         <v>139</v>
       </c>
       <c r="U11" t="s">
         <v>140</v>
       </c>
-      <c r="V11" t="s">
+      <c r="V11" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="W11" t="s">
+      <c r="W11" s="3" t="s">
         <v>142</v>
       </c>
       <c r="X11" t="s">
         <v>143</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Y11" s="3" t="s">
         <v>144</v>
       </c>
       <c r="Z11" s="3" t="s">
@@ -3050,13 +3050,13 @@
       <c r="A12" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>148</v>
       </c>
       <c r="E12" t="s">
@@ -3071,28 +3071,28 @@
       <c r="H12" t="s">
         <v>152</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="3" t="s">
         <v>154</v>
       </c>
       <c r="K12" t="s">
         <v>155</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12" s="3" t="s">
         <v>160</v>
       </c>
       <c r="Q12" t="s">

</xml_diff>

<commit_message>
setup getting ui reports fully working
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C20FDE-B97C-4E86-B3D1-1E4CC24E3DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE4051D-EE82-4CF4-98E3-360998299539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="350">
   <si>
     <t>shopify_orders</t>
   </si>
@@ -1062,6 +1062,15 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>online_store_conversion</t>
+  </si>
+  <si>
+    <t>sales_by_discount</t>
+  </si>
+  <si>
+    <t>shopify_ui</t>
   </si>
 </sst>
 </file>
@@ -1921,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3114,6 +3123,20 @@
         <v>166</v>
       </c>
     </row>
+    <row r="13" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="B13" t="s">
+        <v>347</v>
+      </c>
+      <c r="C13" t="s">
+        <v>348</v>
+      </c>
+      <c r="D13">
+        <v>2792653102</v>
+      </c>
+    </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>167</v>

</xml_diff>

<commit_message>
added active customer count report to shopift
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE4051D-EE82-4CF4-98E3-360998299539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07263D7-32A5-4B1D-890C-1DD4560E3EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="351">
   <si>
     <t>shopify_orders</t>
   </si>
@@ -1071,6 +1071,9 @@
   </si>
   <si>
     <t>shopify_ui</t>
+  </si>
+  <si>
+    <t>customer_count</t>
   </si>
 </sst>
 </file>
@@ -1931,7 +1934,7 @@
   <dimension ref="A1:BJ18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3136,6 +3139,9 @@
       <c r="D13">
         <v>2792653102</v>
       </c>
+      <c r="E13" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">

</xml_diff>

<commit_message>
cleaned up cin7 data to get sales data table
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07263D7-32A5-4B1D-890C-1DD4560E3EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F11ECC-8814-41B3-890A-134EFA1F4E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="324">
   <si>
     <t>shopify_orders</t>
   </si>
@@ -173,57 +173,12 @@
     <t>facebook</t>
   </si>
   <si>
-    <t>page_engaged_users</t>
-  </si>
-  <si>
     <t>page_post_engagements</t>
   </si>
   <si>
     <t>page_consumptions</t>
   </si>
   <si>
-    <t>page_consumptions_by_consumption_type.link clicks</t>
-  </si>
-  <si>
-    <t>page_consumptions_by_consumption_type.other clicks</t>
-  </si>
-  <si>
-    <t>page_consumptions_by_consumption_type.photo view</t>
-  </si>
-  <si>
-    <t>page_consumptions_by_consumption_type.video play</t>
-  </si>
-  <si>
-    <t>page_negative_feedback_by_type.hide clicks</t>
-  </si>
-  <si>
-    <t>page_negative_feedback_by_type.hide all clicks</t>
-  </si>
-  <si>
-    <t>page_negative_feedback_by_type.report spam clicks</t>
-  </si>
-  <si>
-    <t>page_negative_feedback_by_type.unlike page clicks</t>
-  </si>
-  <si>
-    <t>page_positive_feedback_by_type.claim</t>
-  </si>
-  <si>
-    <t>page_positive_feedback_by_type.comment</t>
-  </si>
-  <si>
-    <t>page_positive_feedback_by_type.like</t>
-  </si>
-  <si>
-    <t>page_positive_feedback_by_type.link</t>
-  </si>
-  <si>
-    <t>page_positive_feedback_by_type.other</t>
-  </si>
-  <si>
-    <t>page_positive_feedback_by_type.rsvp</t>
-  </si>
-  <si>
     <t>page_impressions</t>
   </si>
   <si>
@@ -233,60 +188,9 @@
     <t>page_impressions_organic_v2</t>
   </si>
   <si>
-    <t>page_impressions_by_story_type.checkin</t>
-  </si>
-  <si>
-    <t>page_impressions_by_story_type.coupon</t>
-  </si>
-  <si>
-    <t>page_impressions_by_story_type.event</t>
-  </si>
-  <si>
-    <t>page_impressions_by_story_type.fan</t>
-  </si>
-  <si>
-    <t>page_impressions_by_story_type.mention</t>
-  </si>
-  <si>
-    <t>page_impressions_by_story_type.page post</t>
-  </si>
-  <si>
-    <t>page_impressions_by_story_type.question</t>
-  </si>
-  <si>
-    <t>page_impressions_by_story_type.user post</t>
-  </si>
-  <si>
-    <t>page_impressions_by_story_type.other</t>
-  </si>
-  <si>
-    <t>page_posts_impressions</t>
-  </si>
-  <si>
-    <t>page_posts_impressions_paid</t>
-  </si>
-  <si>
-    <t>page_posts_impressions_organic</t>
-  </si>
-  <si>
     <t>page_fans</t>
   </si>
   <si>
-    <t>page_fan_removes</t>
-  </si>
-  <si>
-    <t>page_fans_by_like_source.News Feed</t>
-  </si>
-  <si>
-    <t>page_fans_by_like_source.Page Suggestions</t>
-  </si>
-  <si>
-    <t>page_fans_by_like_source.Restored Likes from Reactivated Accounts</t>
-  </si>
-  <si>
-    <t>page_fans_by_like_source.Search,Your Page</t>
-  </si>
-  <si>
     <t>page_impressions_by_city_unique</t>
   </si>
   <si>
@@ -950,18 +854,12 @@
     <t>page_views_total</t>
   </si>
   <si>
-    <t>page_content_activity_by_action_type_unique</t>
-  </si>
-  <si>
     <t>page_total_actions</t>
   </si>
   <si>
     <t>page_fan_removes_unique</t>
   </si>
   <si>
-    <t>page_fans_by_like_source</t>
-  </si>
-  <si>
     <t>page_fan_adds_unique</t>
   </si>
   <si>
@@ -1074,13 +972,34 @@
   </si>
   <si>
     <t>customer_count</t>
+  </si>
+  <si>
+    <t>cin7_categories</t>
+  </si>
+  <si>
+    <t>GEL NAIL POLISH</t>
+  </si>
+  <si>
+    <t>GIFT CARDS</t>
+  </si>
+  <si>
+    <t>NAIL ART</t>
+  </si>
+  <si>
+    <t>PACKAGING</t>
+  </si>
+  <si>
+    <t>PACKS AND LAMPS</t>
+  </si>
+  <si>
+    <t>TOOLS AND TREATMENTS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1215,13 +1134,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -1405,7 +1317,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.249977111117893"/>
+        <fgColor theme="2" tint="-0.749992370372631"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1575,7 +1487,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1931,10 +1843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ18"/>
+  <dimension ref="A1:BJ19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2015,10 +1927,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>171</v>
+        <v>139</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -2039,7 +1951,7 @@
         <v>9</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>10</v>
@@ -2051,7 +1963,7 @@
         <v>41</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="R1" t="s">
         <v>12</v>
@@ -2060,37 +1972,37 @@
         <v>13</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>174</v>
+        <v>142</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>178</v>
+        <v>146</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>181</v>
+        <v>149</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>182</v>
+        <v>150</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>183</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.3">
@@ -2101,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>16</v>
@@ -2110,16 +2022,16 @@
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>185</v>
+        <v>153</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="H2" t="s">
         <v>17</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>187</v>
+        <v>155</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -2128,157 +2040,157 @@
         <v>19</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>188</v>
+        <v>156</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>189</v>
+        <v>157</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>190</v>
+        <v>158</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>192</v>
+        <v>160</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>194</v>
+        <v>162</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>197</v>
+        <v>165</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>198</v>
+        <v>166</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>200</v>
+        <v>168</v>
       </c>
       <c r="AA2" t="s">
         <v>20</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>201</v>
+        <v>169</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>206</v>
+        <v>174</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>207</v>
+        <v>175</v>
       </c>
       <c r="AI2" t="s">
         <v>21</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>210</v>
+        <v>178</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
       <c r="AV2" s="3" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
       <c r="AX2" s="3" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="AY2" s="3" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
       <c r="AZ2" s="3" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="BA2" s="3" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="BB2" s="3" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="BC2" s="3" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="BD2" s="3" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="BE2" s="3" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="BF2" s="3" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
       <c r="BG2" s="3" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="BH2" s="3" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="BI2" s="3" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="BJ2" s="3" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.3">
@@ -2304,7 +2216,7 @@
         <v>27</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
       <c r="I3" t="s">
         <v>28</v>
@@ -2313,64 +2225,64 @@
         <v>29</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="L3" t="s">
         <v>30</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>238</v>
+        <v>206</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>192</v>
+        <v>160</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>239</v>
+        <v>207</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>240</v>
+        <v>208</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>242</v>
+        <v>210</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>243</v>
+        <v>211</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>244</v>
+        <v>212</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>245</v>
+        <v>213</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>246</v>
+        <v>214</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>247</v>
+        <v>215</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>248</v>
+        <v>216</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>249</v>
+        <v>217</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>250</v>
+        <v>218</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>251</v>
+        <v>219</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>252</v>
+        <v>220</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>253</v>
+        <v>221</v>
       </c>
       <c r="AE3" t="s">
         <v>31</v>
@@ -2379,13 +2291,13 @@
         <v>32</v>
       </c>
       <c r="AG3" s="3" t="s">
-        <v>254</v>
+        <v>222</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>255</v>
+        <v>223</v>
       </c>
       <c r="AI3" s="3" t="s">
-        <v>256</v>
+        <v>224</v>
       </c>
       <c r="AJ3" s="3" t="s">
         <v>33</v>
@@ -2394,7 +2306,7 @@
         <v>34</v>
       </c>
       <c r="AL3" s="3" t="s">
-        <v>257</v>
+        <v>225</v>
       </c>
       <c r="AM3" t="s">
         <v>35</v>
@@ -2403,55 +2315,55 @@
         <v>36</v>
       </c>
       <c r="AO3" s="3" t="s">
-        <v>258</v>
+        <v>226</v>
       </c>
       <c r="AP3" s="3" t="s">
-        <v>259</v>
+        <v>227</v>
       </c>
       <c r="AQ3" s="3" t="s">
-        <v>260</v>
+        <v>228</v>
       </c>
       <c r="AR3" t="s">
         <v>37</v>
       </c>
       <c r="AS3" s="3" t="s">
-        <v>261</v>
+        <v>229</v>
       </c>
       <c r="AT3" s="3" t="s">
-        <v>262</v>
+        <v>230</v>
       </c>
       <c r="AU3" s="3" t="s">
         <v>38</v>
       </c>
       <c r="AV3" s="3" t="s">
-        <v>263</v>
+        <v>231</v>
       </c>
       <c r="AW3" s="3" t="s">
-        <v>264</v>
+        <v>232</v>
       </c>
       <c r="AX3" s="3" t="s">
-        <v>265</v>
+        <v>233</v>
       </c>
       <c r="AY3" s="3" t="s">
-        <v>266</v>
+        <v>234</v>
       </c>
       <c r="AZ3" s="3" t="s">
-        <v>267</v>
+        <v>235</v>
       </c>
       <c r="BA3" s="3" t="s">
-        <v>268</v>
+        <v>236</v>
       </c>
       <c r="BB3" s="3" t="s">
-        <v>269</v>
+        <v>237</v>
       </c>
       <c r="BC3" s="3" t="s">
-        <v>270</v>
+        <v>238</v>
       </c>
       <c r="BD3" s="3" t="s">
-        <v>271</v>
+        <v>239</v>
       </c>
       <c r="BE3" s="3" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.3">
@@ -2468,10 +2380,10 @@
         <v>26</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>272</v>
+        <v>240</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>273</v>
+        <v>241</v>
       </c>
       <c r="G4" t="s">
         <v>41</v>
@@ -2480,7 +2392,7 @@
         <v>13</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>274</v>
+        <v>242</v>
       </c>
       <c r="J4" t="s">
         <v>42</v>
@@ -2489,70 +2401,70 @@
         <v>43</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>44</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>276</v>
+        <v>244</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>277</v>
+        <v>245</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>279</v>
+        <v>247</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>280</v>
+        <v>248</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>281</v>
+        <v>249</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>282</v>
+        <v>250</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>287</v>
+        <v>255</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>288</v>
+        <v>256</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>289</v>
+        <v>257</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>290</v>
+        <v>258</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="AD4" s="3" t="s">
         <v>45</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>292</v>
+        <v>260</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>294</v>
+        <v>262</v>
       </c>
       <c r="AH4" s="3" t="s">
         <v>46</v>
@@ -2561,594 +2473,503 @@
         <v>47</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>295</v>
+        <v>263</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>296</v>
+        <v>264</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="AM4" s="3" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
       <c r="AN4" s="3" t="s">
-        <v>299</v>
+        <v>267</v>
       </c>
       <c r="AO4" s="3" t="s">
         <v>48</v>
       </c>
       <c r="AP4" s="3" t="s">
-        <v>300</v>
+        <v>268</v>
       </c>
       <c r="AQ4" s="3" t="s">
-        <v>301</v>
+        <v>269</v>
       </c>
       <c r="AR4" s="3" t="s">
-        <v>302</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>49</v>
+        <v>317</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>318</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>319</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>320</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>321</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>322</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" t="s">
-        <v>59</v>
-      </c>
-      <c r="L5" t="s">
-        <v>60</v>
-      </c>
-      <c r="M5" t="s">
-        <v>61</v>
-      </c>
-      <c r="N5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>65</v>
-      </c>
-      <c r="R5" t="s">
-        <v>66</v>
-      </c>
-      <c r="S5" t="s">
-        <v>67</v>
-      </c>
-      <c r="T5" t="s">
-        <v>68</v>
-      </c>
-      <c r="U5" t="s">
-        <v>69</v>
-      </c>
-      <c r="V5" t="s">
-        <v>70</v>
-      </c>
-      <c r="W5" t="s">
-        <v>71</v>
-      </c>
-      <c r="X5" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE5" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF5" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AG5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AI5" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>84</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>86</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>88</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>89</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>91</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>303</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>304</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>305</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>306</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>307</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>308</v>
-      </c>
-      <c r="AY5" t="s">
-        <v>309</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>310</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>50</v>
-      </c>
-      <c r="BB5" t="s">
-        <v>69</v>
-      </c>
-      <c r="BC5" t="s">
-        <v>311</v>
-      </c>
-      <c r="BD5" t="s">
-        <v>312</v>
-      </c>
-      <c r="BE5" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF5" t="s">
-        <v>308</v>
-      </c>
-      <c r="BG5" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>314</v>
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>346</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>343</v>
+        <v>53</v>
       </c>
       <c r="F6" t="s">
-        <v>344</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>345</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>333</v>
+        <v>56</v>
       </c>
       <c r="I6" t="s">
-        <v>334</v>
+        <v>57</v>
       </c>
       <c r="J6" t="s">
-        <v>335</v>
+        <v>58</v>
       </c>
       <c r="K6" t="s">
-        <v>336</v>
-      </c>
-      <c r="L6" t="s">
-        <v>337</v>
-      </c>
-      <c r="M6" t="s">
-        <v>338</v>
-      </c>
-      <c r="N6" t="s">
-        <v>339</v>
-      </c>
-      <c r="O6" t="s">
-        <v>340</v>
-      </c>
-      <c r="P6" t="s">
-        <v>341</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>342</v>
+        <v>59</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>93</v>
+        <v>298</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>314</v>
+        <v>280</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>312</v>
       </c>
       <c r="E7" t="s">
-        <v>96</v>
+        <v>309</v>
       </c>
       <c r="F7" t="s">
-        <v>97</v>
+        <v>310</v>
       </c>
       <c r="G7" t="s">
-        <v>98</v>
+        <v>311</v>
       </c>
       <c r="H7" t="s">
-        <v>99</v>
+        <v>299</v>
       </c>
       <c r="I7" t="s">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="J7" t="s">
-        <v>101</v>
+        <v>301</v>
       </c>
       <c r="K7" t="s">
-        <v>102</v>
+        <v>302</v>
       </c>
       <c r="L7" t="s">
-        <v>103</v>
+        <v>303</v>
       </c>
       <c r="M7" t="s">
-        <v>104</v>
+        <v>304</v>
+      </c>
+      <c r="N7" t="s">
+        <v>305</v>
+      </c>
+      <c r="O7" t="s">
+        <v>306</v>
+      </c>
+      <c r="P7" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" t="s">
-        <v>89</v>
+        <v>61</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>280</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>64</v>
+      </c>
+      <c r="F8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L8" t="s">
+        <v>71</v>
+      </c>
+      <c r="M8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F9" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H9" t="s">
-        <v>113</v>
-      </c>
-      <c r="I9" t="s">
-        <v>114</v>
-      </c>
-      <c r="J9" t="s">
-        <v>115</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="U9" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="V9" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="W9" s="3" t="s">
-        <v>327</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>1</v>
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="E10" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="F10" t="s">
-        <v>97</v>
+        <v>79</v>
+      </c>
+      <c r="G10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" t="s">
-        <v>122</v>
+        <v>84</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="E11" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="F11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G11" t="s">
-        <v>126</v>
-      </c>
-      <c r="H11" t="s">
-        <v>127</v>
-      </c>
-      <c r="I11" t="s">
-        <v>128</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="M11" t="s">
-        <v>132</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="O11" t="s">
-        <v>134</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>136</v>
-      </c>
-      <c r="R11" t="s">
-        <v>137</v>
-      </c>
-      <c r="S11" t="s">
-        <v>138</v>
-      </c>
-      <c r="T11" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="U11" t="s">
-        <v>140</v>
-      </c>
-      <c r="V11" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="W11" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="X11" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y11" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z11" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="AA11" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="AB11" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="AC11" s="3" t="s">
-        <v>331</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>148</v>
+        <v>88</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" t="s">
+        <v>91</v>
       </c>
       <c r="E12" t="s">
-        <v>149</v>
+        <v>92</v>
       </c>
       <c r="F12" t="s">
-        <v>150</v>
+        <v>93</v>
       </c>
       <c r="G12" t="s">
-        <v>151</v>
+        <v>94</v>
       </c>
       <c r="H12" t="s">
-        <v>152</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>153</v>
+        <v>95</v>
+      </c>
+      <c r="I12" t="s">
+        <v>96</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="K12" t="s">
-        <v>155</v>
+        <v>97</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>157</v>
+        <v>99</v>
+      </c>
+      <c r="M12" t="s">
+        <v>100</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>159</v>
+        <v>101</v>
+      </c>
+      <c r="O12" t="s">
+        <v>102</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="Q12" t="s">
-        <v>161</v>
+        <v>104</v>
       </c>
       <c r="R12" t="s">
-        <v>162</v>
+        <v>105</v>
       </c>
       <c r="S12" t="s">
-        <v>163</v>
-      </c>
-      <c r="T12" t="s">
-        <v>164</v>
+        <v>106</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="U12" t="s">
-        <v>165</v>
-      </c>
-      <c r="V12" t="s">
-        <v>166</v>
+        <v>108</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="X12" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z12" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="AC12" s="3" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="B13" t="s">
-        <v>347</v>
-      </c>
-      <c r="C13" t="s">
-        <v>348</v>
-      </c>
-      <c r="D13">
+        <v>113</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G13" t="s">
+        <v>119</v>
+      </c>
+      <c r="H13" t="s">
+        <v>120</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="K13" t="s">
+        <v>123</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>129</v>
+      </c>
+      <c r="R13" t="s">
+        <v>130</v>
+      </c>
+      <c r="S13" t="s">
+        <v>131</v>
+      </c>
+      <c r="T13" t="s">
+        <v>132</v>
+      </c>
+      <c r="U13" t="s">
+        <v>133</v>
+      </c>
+      <c r="V13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B14" t="s">
+        <v>313</v>
+      </c>
+      <c r="C14" t="s">
+        <v>314</v>
+      </c>
+      <c r="D14">
         <v>2792653102</v>
       </c>
-      <c r="E13" t="s">
-        <v>350</v>
+      <c r="E14" t="s">
+        <v>316</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>169</v>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -3169,13 +2990,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cin7 data now matching the original tables
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F11ECC-8814-41B3-890A-134EFA1F4E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3843D5-4A63-4E26-BC40-717CFDD54779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1846,7 +1846,7 @@
   <dimension ref="A1:BJ19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2508,19 +2508,19 @@
         <v>318</v>
       </c>
       <c r="C5" t="s">
+        <v>320</v>
+      </c>
+      <c r="D5" t="s">
+        <v>322</v>
+      </c>
+      <c r="E5" t="s">
+        <v>323</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="D5" t="s">
-        <v>320</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G5" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="F5" t="s">
-        <v>322</v>
-      </c>
-      <c r="G5" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
shopify now gets more customer data
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3843D5-4A63-4E26-BC40-717CFDD54779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BFDE66-A9DE-4619-A32E-28D1DA9FA22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="325">
   <si>
     <t>shopify_orders</t>
   </si>
@@ -993,6 +993,9 @@
   </si>
   <si>
     <t>TOOLS AND TREATMENTS</t>
+  </si>
+  <si>
+    <t>sales_over_time</t>
   </si>
 </sst>
 </file>
@@ -1846,7 +1849,7 @@
   <dimension ref="A1:BJ19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2963,6 +2966,9 @@
       <c r="E14" t="s">
         <v>316</v>
       </c>
+      <c r="F14" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">

</xml_diff>

<commit_message>
Changed to stop error on blank excel changed to refresh for finding shopify table updated headers updated for more insta info updated cin7 data
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BFDE66-A9DE-4619-A32E-28D1DA9FA22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABE320A-EEBC-4EDF-AF3B-D5AF91B9A345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="324">
   <si>
     <t>shopify_orders</t>
   </si>
@@ -282,9 +282,6 @@
   </si>
   <si>
     <t>caption</t>
-  </si>
-  <si>
-    <t>like_count</t>
   </si>
   <si>
     <t>google_metrics</t>
@@ -1849,7 +1846,7 @@
   <dimension ref="A1:BJ19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1930,10 +1927,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -1954,7 +1951,7 @@
         <v>9</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>10</v>
@@ -1966,7 +1963,7 @@
         <v>41</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R1" t="s">
         <v>12</v>
@@ -1975,37 +1972,37 @@
         <v>13</v>
       </c>
       <c r="T1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="AB1" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC1" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.3">
@@ -2016,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>16</v>
@@ -2025,16 +2022,16 @@
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="H2" t="s">
         <v>17</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -2043,157 +2040,157 @@
         <v>19</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="AA2" t="s">
         <v>20</v>
       </c>
       <c r="AB2" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="AC2" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="AI2" t="s">
         <v>21</v>
       </c>
       <c r="AJ2" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="AK2" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AN2" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AO2" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AP2" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AR2" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AS2" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AT2" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AU2" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AV2" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="AV2" s="3" t="s">
+      <c r="AW2" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AX2" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="AX2" s="3" t="s">
+      <c r="AY2" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="AY2" s="3" t="s">
+      <c r="AZ2" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="AZ2" s="3" t="s">
+      <c r="BA2" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="BA2" s="3" t="s">
+      <c r="BB2" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="BB2" s="3" t="s">
+      <c r="BC2" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="BC2" s="3" t="s">
+      <c r="BD2" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="BD2" s="3" t="s">
+      <c r="BE2" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="BE2" s="3" t="s">
+      <c r="BF2" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="BF2" s="3" t="s">
+      <c r="BG2" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="BG2" s="3" t="s">
+      <c r="BH2" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="BH2" s="3" t="s">
+      <c r="BI2" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="BI2" s="3" t="s">
+      <c r="BJ2" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="BJ2" s="3" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.3">
@@ -2219,7 +2216,7 @@
         <v>27</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I3" t="s">
         <v>28</v>
@@ -2228,64 +2225,64 @@
         <v>29</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L3" t="s">
         <v>30</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="AE3" t="s">
         <v>31</v>
@@ -2294,13 +2291,13 @@
         <v>32</v>
       </c>
       <c r="AG3" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="AH3" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="AH3" s="3" t="s">
+      <c r="AI3" s="3" t="s">
         <v>223</v>
-      </c>
-      <c r="AI3" s="3" t="s">
-        <v>224</v>
       </c>
       <c r="AJ3" s="3" t="s">
         <v>33</v>
@@ -2309,7 +2306,7 @@
         <v>34</v>
       </c>
       <c r="AL3" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AM3" t="s">
         <v>35</v>
@@ -2318,55 +2315,55 @@
         <v>36</v>
       </c>
       <c r="AO3" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AP3" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="AP3" s="3" t="s">
+      <c r="AQ3" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="AQ3" s="3" t="s">
-        <v>228</v>
       </c>
       <c r="AR3" t="s">
         <v>37</v>
       </c>
       <c r="AS3" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="AT3" s="3" t="s">
         <v>229</v>
-      </c>
-      <c r="AT3" s="3" t="s">
-        <v>230</v>
       </c>
       <c r="AU3" s="3" t="s">
         <v>38</v>
       </c>
       <c r="AV3" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="AW3" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="AW3" s="3" t="s">
+      <c r="AX3" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="AX3" s="3" t="s">
+      <c r="AY3" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="AY3" s="3" t="s">
+      <c r="AZ3" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="AZ3" s="3" t="s">
+      <c r="BA3" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="BA3" s="3" t="s">
+      <c r="BB3" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="BB3" s="3" t="s">
+      <c r="BC3" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="BC3" s="3" t="s">
+      <c r="BD3" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="BD3" s="3" t="s">
-        <v>239</v>
-      </c>
       <c r="BE3" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.3">
@@ -2383,10 +2380,10 @@
         <v>26</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="G4" t="s">
         <v>41</v>
@@ -2395,7 +2392,7 @@
         <v>13</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J4" t="s">
         <v>42</v>
@@ -2404,70 +2401,70 @@
         <v>43</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>44</v>
       </c>
       <c r="N4" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="AD4" s="3" t="s">
         <v>45</v>
       </c>
       <c r="AE4" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="AF4" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>262</v>
       </c>
       <c r="AH4" s="3" t="s">
         <v>46</v>
@@ -2476,54 +2473,54 @@
         <v>47</v>
       </c>
       <c r="AJ4" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="AK4" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>266</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>267</v>
       </c>
       <c r="AO4" s="3" t="s">
         <v>48</v>
       </c>
       <c r="AP4" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="AQ4" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>269</v>
-      </c>
-      <c r="AR4" s="3" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B5" t="s">
         <v>317</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>319</v>
+      </c>
+      <c r="D5" t="s">
+        <v>321</v>
+      </c>
+      <c r="E5" t="s">
+        <v>322</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" s="3" t="s">
         <v>320</v>
-      </c>
-      <c r="D5" t="s">
-        <v>322</v>
-      </c>
-      <c r="E5" t="s">
-        <v>323</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.3">
@@ -2533,7 +2530,7 @@
       <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D6" t="s">
@@ -2560,88 +2557,88 @@
       <c r="K6" t="s">
         <v>59</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" t="s">
         <v>60</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" t="s">
+        <v>270</v>
+      </c>
+      <c r="N6" t="s">
         <v>271</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" t="s">
         <v>272</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" t="s">
         <v>273</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" t="s">
         <v>274</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" t="s">
         <v>275</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" t="s">
         <v>276</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="T6" t="s">
         <v>277</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="U6" t="s">
         <v>278</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D7" t="s">
-        <v>312</v>
-      </c>
-      <c r="E7" t="s">
+        <v>311</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>310</v>
       </c>
-      <c r="G7" t="s">
-        <v>311</v>
-      </c>
       <c r="H7" t="s">
+        <v>298</v>
+      </c>
+      <c r="I7" t="s">
         <v>299</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>300</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>301</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>302</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>303</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>304</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>305</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>306</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>307</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.3">
@@ -2652,7 +2649,7 @@
         <v>62</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
@@ -2721,7 +2718,7 @@
       <c r="F10" t="s">
         <v>79</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="3" t="s">
         <v>80</v>
       </c>
       <c r="H10" t="s">
@@ -2734,43 +2731,43 @@
         <v>83</v>
       </c>
       <c r="K10" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="P10" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="Q10" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="Q10" s="3" t="s">
+      <c r="R10" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="R10" s="3" t="s">
+      <c r="S10" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="S10" s="3" t="s">
+      <c r="T10" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="T10" s="3" t="s">
+      <c r="U10" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="U10" s="3" t="s">
+      <c r="V10" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="V10" s="3" t="s">
+      <c r="W10" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="W10" s="3" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.3">
@@ -2787,195 +2784,201 @@
         <v>86</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>282</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>283</v>
+      </c>
+      <c r="G11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s">
         <v>88</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>89</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>90</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>91</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>92</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>93</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>94</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>95</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="K12" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="L12" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="M12" t="s">
         <v>99</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="O12" t="s">
         <v>101</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="Q12" t="s">
         <v>103</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>104</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>105</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="T12" s="3" t="s">
+      <c r="U12" t="s">
         <v>107</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="V12" s="3" t="s">
+      <c r="W12" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="W12" s="3" t="s">
+      <c r="X12" t="s">
         <v>110</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="Y12" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="Z12" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="AA12" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="AA12" s="3" t="s">
+      <c r="AB12" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="AB12" s="3" t="s">
+      <c r="AC12" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="AC12" s="3" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" t="s">
         <v>116</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>117</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>118</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>119</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="K13" t="s">
         <v>122</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="M13" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="N13" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="O13" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="P13" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="P13" s="3" t="s">
+      <c r="Q13" t="s">
         <v>128</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>129</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>130</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>131</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>132</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>133</v>
-      </c>
-      <c r="V13" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B14" t="s">
+        <v>312</v>
+      </c>
+      <c r="C14" t="s">
         <v>313</v>
-      </c>
-      <c r="C14" t="s">
-        <v>314</v>
       </c>
       <c r="D14">
         <v>2792653102</v>
       </c>
       <c r="E14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2996,13 +2999,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated shopify to add orders and revenue to conversion rate sheet
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABE320A-EEBC-4EDF-AF3B-D5AF91B9A345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AE4B2E-8858-4366-9E1D-4A81C173B875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="headers" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="325">
   <si>
     <t>shopify_orders</t>
   </si>
@@ -993,6 +993,9 @@
   </si>
   <si>
     <t>sales_over_time</t>
+  </si>
+  <si>
+    <t>orders_over_time</t>
   </si>
 </sst>
 </file>
@@ -1845,8 +1848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2972,6 +2975,9 @@
       <c r="F14" t="s">
         <v>323</v>
       </c>
+      <c r="G14" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">

</xml_diff>

<commit_message>
starshipit report cut down to a week where requested
new headers added

employee map added for starshipit report
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AE4B2E-8858-4366-9E1D-4A81C173B875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64ECBB9-1988-42A5-A52A-2490976A3C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="headers" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="337">
   <si>
     <t>shopify_orders</t>
   </si>
@@ -996,6 +996,42 @@
   </si>
   <si>
     <t>orders_over_time</t>
+  </si>
+  <si>
+    <t>starshipit_ui</t>
+  </si>
+  <si>
+    <t>Order Date</t>
+  </si>
+  <si>
+    <t>Printed Date</t>
+  </si>
+  <si>
+    <t>Delivered Date</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Carrier</t>
+  </si>
+  <si>
+    <t>Package Sent</t>
+  </si>
+  <si>
+    <t>AccountName</t>
+  </si>
+  <si>
+    <t>Item Skus</t>
+  </si>
+  <si>
+    <t>tracking_short_status</t>
+  </si>
+  <si>
+    <t>tracking_number</t>
+  </si>
+  <si>
+    <t>results.last_updated_date</t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1361,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1440,6 +1476,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1490,7 +1535,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1846,10 +1891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ19"/>
+  <dimension ref="A1:BJ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BH26" sqref="BH26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2198,455 +2243,440 @@
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>22</v>
+        <v>325</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="I3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="L3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="AI3" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO3" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="AP3" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="AQ3" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AS3" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="AT3" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="AU3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AV3" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="AW3" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="AX3" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="AY3" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="AZ3" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="BA3" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="BB3" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="BC3" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="BD3" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="BE3" s="3" t="s">
-        <v>125</v>
+        <v>326</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>240</v>
-      </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>241</v>
+        <v>202</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>242</v>
+        <v>29</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L4" t="s">
+        <v>30</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>44</v>
+        <v>204</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>243</v>
+        <v>205</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>244</v>
+        <v>159</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>245</v>
+        <v>206</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>246</v>
+        <v>207</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>247</v>
+        <v>208</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>248</v>
+        <v>209</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>249</v>
+        <v>210</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>250</v>
+        <v>211</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>251</v>
+        <v>212</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>252</v>
+        <v>213</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>253</v>
+        <v>214</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>254</v>
+        <v>215</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>255</v>
+        <v>216</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>256</v>
+        <v>217</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>257</v>
+        <v>218</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>258</v>
+        <v>219</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>260</v>
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>32</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>261</v>
+        <v>221</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>46</v>
+        <v>222</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>47</v>
+        <v>223</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>262</v>
+        <v>33</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>263</v>
+        <v>34</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>265</v>
+        <v>224</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>35</v>
       </c>
       <c r="AN4" s="3" t="s">
-        <v>266</v>
+        <v>36</v>
       </c>
       <c r="AO4" s="3" t="s">
-        <v>48</v>
+        <v>225</v>
       </c>
       <c r="AP4" s="3" t="s">
-        <v>267</v>
+        <v>226</v>
       </c>
       <c r="AQ4" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="AR4" s="3" t="s">
-        <v>269</v>
+        <v>227</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS4" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="AT4" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="AU4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AV4" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="AW4" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="AX4" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="AY4" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="AZ4" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="BA4" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="BB4" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="BC4" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="BD4" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="BE4" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="BF4" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="BG4" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="BH4" s="2" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="B5" t="s">
-        <v>317</v>
-      </c>
-      <c r="C5" t="s">
-        <v>319</v>
-      </c>
-      <c r="D5" t="s">
-        <v>321</v>
-      </c>
-      <c r="E5" t="s">
-        <v>322</v>
+        <v>39</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>320</v>
+        <v>240</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="J5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="AH5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ5" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="AK5" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="AL5" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="AM5" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="AN5" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="AO5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP5" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="AQ5" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="AR5" s="3" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>49</v>
+        <v>316</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>51</v>
+        <v>317</v>
+      </c>
+      <c r="C6" t="s">
+        <v>319</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>321</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K6" t="s">
-        <v>59</v>
-      </c>
-      <c r="L6" t="s">
-        <v>60</v>
-      </c>
-      <c r="M6" t="s">
-        <v>270</v>
-      </c>
-      <c r="N6" t="s">
-        <v>271</v>
-      </c>
-      <c r="O6" t="s">
-        <v>272</v>
-      </c>
-      <c r="P6" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>274</v>
-      </c>
-      <c r="R6" t="s">
-        <v>275</v>
-      </c>
-      <c r="S6" t="s">
-        <v>276</v>
-      </c>
-      <c r="T6" t="s">
-        <v>277</v>
-      </c>
-      <c r="U6" t="s">
-        <v>278</v>
+        <v>322</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>62</v>
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>279</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>311</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>309</v>
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>310</v>
+        <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>298</v>
+        <v>56</v>
       </c>
       <c r="I7" t="s">
-        <v>299</v>
+        <v>57</v>
       </c>
       <c r="J7" t="s">
-        <v>300</v>
+        <v>58</v>
       </c>
       <c r="K7" t="s">
-        <v>301</v>
+        <v>59</v>
       </c>
       <c r="L7" t="s">
-        <v>302</v>
+        <v>60</v>
       </c>
       <c r="M7" t="s">
-        <v>303</v>
+        <v>270</v>
       </c>
       <c r="N7" t="s">
-        <v>304</v>
+        <v>271</v>
       </c>
       <c r="O7" t="s">
-        <v>305</v>
+        <v>272</v>
       </c>
       <c r="P7" t="s">
-        <v>306</v>
+        <v>273</v>
       </c>
       <c r="Q7" t="s">
-        <v>307</v>
+        <v>274</v>
+      </c>
+      <c r="R7" t="s">
+        <v>275</v>
+      </c>
+      <c r="S7" t="s">
+        <v>276</v>
+      </c>
+      <c r="T7" t="s">
+        <v>277</v>
+      </c>
+      <c r="U7" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>61</v>
+        <v>297</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>62</v>
@@ -2655,335 +2685,388 @@
         <v>279</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" t="s">
-        <v>65</v>
+        <v>311</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>309</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
+        <v>310</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>298</v>
       </c>
       <c r="I8" t="s">
-        <v>68</v>
+        <v>299</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>300</v>
       </c>
       <c r="K8" t="s">
-        <v>70</v>
+        <v>301</v>
       </c>
       <c r="L8" t="s">
-        <v>71</v>
+        <v>302</v>
       </c>
       <c r="M8" t="s">
-        <v>72</v>
+        <v>303</v>
+      </c>
+      <c r="N8" t="s">
+        <v>304</v>
+      </c>
+      <c r="O8" t="s">
+        <v>305</v>
+      </c>
+      <c r="P8" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" t="s">
-        <v>57</v>
+        <v>61</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>279</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>64</v>
+      </c>
+      <c r="F9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" t="s">
+        <v>71</v>
+      </c>
+      <c r="M9" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" t="s">
-        <v>81</v>
-      </c>
-      <c r="I10" t="s">
-        <v>82</v>
-      </c>
-      <c r="J10" t="s">
-        <v>83</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="T10" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="U10" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="V10" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="W10" s="3" t="s">
-        <v>292</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>1</v>
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="F11" t="s">
+      <c r="N11" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="G11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="O11" s="3" t="s">
         <v>284</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E12" t="s">
-        <v>91</v>
+        <v>282</v>
       </c>
       <c r="F12" t="s">
-        <v>92</v>
+        <v>283</v>
       </c>
       <c r="G12" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="H12" t="s">
-        <v>94</v>
-      </c>
-      <c r="I12" t="s">
-        <v>95</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="M12" t="s">
-        <v>99</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="O12" t="s">
-        <v>101</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>103</v>
-      </c>
-      <c r="R12" t="s">
-        <v>104</v>
-      </c>
-      <c r="S12" t="s">
-        <v>105</v>
-      </c>
-      <c r="T12" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="U12" t="s">
-        <v>107</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="W12" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="X12" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y12" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="Z12" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="AA12" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="AB12" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="AC12" s="3" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>115</v>
+        <v>87</v>
+      </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" t="s">
+        <v>90</v>
       </c>
       <c r="E13" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="G13" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="H13" t="s">
-        <v>119</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>120</v>
+        <v>94</v>
+      </c>
+      <c r="I13" t="s">
+        <v>95</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="K13" t="s">
-        <v>122</v>
+        <v>96</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>124</v>
+        <v>98</v>
+      </c>
+      <c r="M13" t="s">
+        <v>99</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>126</v>
+        <v>100</v>
+      </c>
+      <c r="O13" t="s">
+        <v>101</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="Q13" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="R13" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="S13" t="s">
-        <v>130</v>
-      </c>
-      <c r="T13" t="s">
-        <v>131</v>
+        <v>105</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="U13" t="s">
-        <v>132</v>
-      </c>
-      <c r="V13" t="s">
-        <v>133</v>
+        <v>107</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="X13" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z13" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC13" s="3" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="K14" t="s">
+        <v>122</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>128</v>
+      </c>
+      <c r="R14" t="s">
+        <v>129</v>
+      </c>
+      <c r="S14" t="s">
+        <v>130</v>
+      </c>
+      <c r="T14" t="s">
+        <v>131</v>
+      </c>
+      <c r="U14" t="s">
+        <v>132</v>
+      </c>
+      <c r="V14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>312</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>313</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>2792653102</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>315</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>323</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>136</v>
       </c>
     </row>

</xml_diff>

<commit_message>
staff mappings now combine table
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64ECBB9-1988-42A5-A52A-2490976A3C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F23CE9C-F293-42A0-BFB4-9F8F957B7F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1893,8 +1893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BH26" sqref="BH26"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2711,7 +2711,7 @@
       <c r="L8" t="s">
         <v>302</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="3" t="s">
         <v>303</v>
       </c>
       <c r="N8" t="s">

</xml_diff>

<commit_message>
setup update files to be more robust aged report is being fully fetched and trimmed
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E65F9F-064D-4730-86E2-771417B720D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8929FE9-522C-4170-B34B-EA43F49FD0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="345">
   <si>
     <t>shopify_orders</t>
   </si>
@@ -1044,6 +1044,18 @@
   </si>
   <si>
     <t>GEL LAMP PACKS</t>
+  </si>
+  <si>
+    <t>Barcode</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>cin7_aged_trim</t>
   </si>
 </sst>
 </file>
@@ -1903,10 +1915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ20"/>
+  <dimension ref="A1:BJ21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2635,125 +2647,86 @@
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>49</v>
+        <v>344</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>51</v>
+        <v>341</v>
+      </c>
+      <c r="C7" t="s">
+        <v>342</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" t="s">
-        <v>57</v>
-      </c>
-      <c r="J7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K7" t="s">
-        <v>59</v>
-      </c>
-      <c r="L7" t="s">
-        <v>60</v>
-      </c>
-      <c r="M7" t="s">
-        <v>270</v>
-      </c>
-      <c r="N7" t="s">
-        <v>271</v>
-      </c>
-      <c r="O7" t="s">
-        <v>272</v>
-      </c>
-      <c r="P7" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>274</v>
-      </c>
-      <c r="R7" t="s">
-        <v>275</v>
-      </c>
-      <c r="S7" t="s">
-        <v>276</v>
-      </c>
-      <c r="T7" t="s">
-        <v>277</v>
-      </c>
-      <c r="U7" t="s">
-        <v>278</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>62</v>
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>279</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>311</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>309</v>
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>310</v>
+        <v>55</v>
       </c>
       <c r="H8" t="s">
-        <v>298</v>
+        <v>56</v>
       </c>
       <c r="I8" t="s">
-        <v>299</v>
+        <v>57</v>
       </c>
       <c r="J8" t="s">
-        <v>300</v>
+        <v>58</v>
       </c>
       <c r="K8" t="s">
-        <v>301</v>
+        <v>59</v>
       </c>
       <c r="L8" t="s">
-        <v>302</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>303</v>
+        <v>60</v>
+      </c>
+      <c r="M8" t="s">
+        <v>270</v>
       </c>
       <c r="N8" t="s">
-        <v>304</v>
+        <v>271</v>
       </c>
       <c r="O8" t="s">
-        <v>305</v>
+        <v>272</v>
       </c>
       <c r="P8" t="s">
-        <v>306</v>
+        <v>273</v>
       </c>
       <c r="Q8" t="s">
-        <v>307</v>
+        <v>274</v>
+      </c>
+      <c r="R8" t="s">
+        <v>275</v>
+      </c>
+      <c r="S8" t="s">
+        <v>276</v>
+      </c>
+      <c r="T8" t="s">
+        <v>277</v>
+      </c>
+      <c r="U8" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>61</v>
+        <v>297</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>62</v>
@@ -2762,335 +2735,391 @@
         <v>279</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" t="s">
-        <v>65</v>
+        <v>311</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>309</v>
       </c>
       <c r="G9" t="s">
-        <v>66</v>
+        <v>310</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>298</v>
       </c>
       <c r="I9" t="s">
-        <v>68</v>
+        <v>299</v>
       </c>
       <c r="J9" t="s">
-        <v>69</v>
+        <v>300</v>
       </c>
       <c r="K9" t="s">
-        <v>70</v>
+        <v>301</v>
       </c>
       <c r="L9" t="s">
-        <v>71</v>
-      </c>
-      <c r="M9" t="s">
-        <v>72</v>
+        <v>302</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="N9" t="s">
+        <v>304</v>
+      </c>
+      <c r="O9" t="s">
+        <v>305</v>
+      </c>
+      <c r="P9" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" t="s">
-        <v>57</v>
+        <v>61</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>279</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>64</v>
+      </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" t="s">
+        <v>71</v>
+      </c>
+      <c r="M10" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H11" t="s">
-        <v>81</v>
-      </c>
-      <c r="I11" t="s">
-        <v>82</v>
-      </c>
-      <c r="J11" t="s">
-        <v>83</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="R11" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="S11" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="T11" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="U11" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="V11" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="W11" s="3" t="s">
-        <v>292</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>1</v>
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J12" t="s">
+        <v>83</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="F12" t="s">
+      <c r="N12" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="G12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="O12" s="3" t="s">
         <v>284</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E13" t="s">
-        <v>91</v>
+        <v>282</v>
       </c>
       <c r="F13" t="s">
-        <v>92</v>
+        <v>283</v>
       </c>
       <c r="G13" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="H13" t="s">
-        <v>94</v>
-      </c>
-      <c r="I13" t="s">
-        <v>95</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="M13" t="s">
-        <v>99</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="O13" t="s">
-        <v>101</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>103</v>
-      </c>
-      <c r="R13" t="s">
-        <v>104</v>
-      </c>
-      <c r="S13" t="s">
-        <v>105</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="U13" t="s">
-        <v>107</v>
-      </c>
-      <c r="V13" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="W13" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="X13" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y13" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="Z13" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="AA13" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="AB13" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="AC13" s="3" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>115</v>
+        <v>87</v>
+      </c>
+      <c r="B14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" t="s">
+        <v>90</v>
       </c>
       <c r="E14" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="F14" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="G14" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="H14" t="s">
-        <v>119</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>120</v>
+        <v>94</v>
+      </c>
+      <c r="I14" t="s">
+        <v>95</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="K14" t="s">
-        <v>122</v>
+        <v>96</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>124</v>
+        <v>98</v>
+      </c>
+      <c r="M14" t="s">
+        <v>99</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>126</v>
+        <v>100</v>
+      </c>
+      <c r="O14" t="s">
+        <v>101</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="Q14" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="R14" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="S14" t="s">
-        <v>130</v>
-      </c>
-      <c r="T14" t="s">
-        <v>131</v>
+        <v>105</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="U14" t="s">
-        <v>132</v>
-      </c>
-      <c r="V14" t="s">
-        <v>133</v>
+        <v>107</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="X14" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z14" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="AA14" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="AB14" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC14" s="3" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" t="s">
+        <v>118</v>
+      </c>
+      <c r="H15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="K15" t="s">
+        <v>122</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>128</v>
+      </c>
+      <c r="R15" t="s">
+        <v>129</v>
+      </c>
+      <c r="S15" t="s">
+        <v>130</v>
+      </c>
+      <c r="T15" t="s">
+        <v>131</v>
+      </c>
+      <c r="U15" t="s">
+        <v>132</v>
+      </c>
+      <c r="V15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>312</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>313</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>2792653102</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>315</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" t="s">
         <v>322</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>136</v>
       </c>
     </row>

</xml_diff>

<commit_message>
output saves into date folders updated to get open orders count updated to get correct shipping total cost
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8929FE9-522C-4170-B34B-EA43F49FD0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5137BC74-C5DD-4EDD-9547-9B1A8973B17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="350">
   <si>
     <t>shopify_orders</t>
   </si>
@@ -1056,6 +1056,21 @@
   </si>
   <si>
     <t>cin7_aged_trim</t>
+  </si>
+  <si>
+    <t>shipping</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>Suburb</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Postcode</t>
   </si>
 </sst>
 </file>
@@ -1554,12 +1569,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1917,8 +1935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2293,6 +2311,21 @@
       <c r="I3" s="2" t="s">
         <v>332</v>
       </c>
+      <c r="J3" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -3106,10 +3139,13 @@
         <v>315</v>
       </c>
       <c r="F16" t="s">
+        <v>323</v>
+      </c>
+      <c r="G16" t="s">
         <v>322</v>
       </c>
-      <c r="G16" t="s">
-        <v>323</v>
+      <c r="H16" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
getting full stats for instagram images and videos
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5137BC74-C5DD-4EDD-9547-9B1A8973B17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901E6BD0-626B-41BB-98DB-BA2A883EAB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="351">
   <si>
     <t>shopify_orders</t>
   </si>
@@ -1071,6 +1071,9 @@
   </si>
   <si>
     <t>Postcode</t>
+  </si>
+  <si>
+    <t>media_type</t>
   </si>
 </sst>
 </file>
@@ -1935,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2964,6 +2967,12 @@
       <c r="H13" t="s">
         <v>284</v>
       </c>
+      <c r="I13" t="s">
+        <v>350</v>
+      </c>
+      <c r="J13" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">

</xml_diff>

<commit_message>
cleaned discounts with mapping cleaned products with cleaning function updated aged products retrieving to be more robust
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901E6BD0-626B-41BB-98DB-BA2A883EAB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFA19D1-CDD7-4E67-8405-338E2EDE7ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="357">
   <si>
     <t>shopify_orders</t>
   </si>
@@ -1074,6 +1074,24 @@
   </si>
   <si>
     <t>media_type</t>
+  </si>
+  <si>
+    <t>Packs</t>
+  </si>
+  <si>
+    <t>Consumables</t>
+  </si>
+  <si>
+    <t>Production Charges</t>
+  </si>
+  <si>
+    <t>Replacement</t>
+  </si>
+  <si>
+    <t>Packaging</t>
+  </si>
+  <si>
+    <t>Booklet</t>
   </si>
 </sst>
 </file>
@@ -1938,8 +1956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2694,6 +2712,24 @@
       <c r="D7" t="s">
         <v>343</v>
       </c>
+      <c r="E7" t="s">
+        <v>351</v>
+      </c>
+      <c r="F7" t="s">
+        <v>352</v>
+      </c>
+      <c r="G7" t="s">
+        <v>353</v>
+      </c>
+      <c r="H7" t="s">
+        <v>354</v>
+      </c>
+      <c r="I7" t="s">
+        <v>355</v>
+      </c>
+      <c r="J7" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">

</xml_diff>

<commit_message>
week 12 output, working but needs some cleanup in a few spots, marked with todo
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9B599A-6ABC-49BB-AD35-FDE654DBCCE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFD1630-EDA4-4DC6-8338-4E818E0DFDA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="headers" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="366">
   <si>
     <t>shopify_orders</t>
   </si>
@@ -1031,91 +1031,94 @@
     <t>results.last_updated_date</t>
   </si>
   <si>
+    <t>PRODUCTION CHARGES</t>
+  </si>
+  <si>
+    <t>LIMITED EDITION</t>
+  </si>
+  <si>
+    <t>CHROME POWDER</t>
+  </si>
+  <si>
+    <t>GEL LAMP PACKS</t>
+  </si>
+  <si>
+    <t>Barcode</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>cin7_aged_trim</t>
+  </si>
+  <si>
+    <t>shipping</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>Suburb</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>media_type</t>
+  </si>
+  <si>
+    <t>Packs</t>
+  </si>
+  <si>
+    <t>Consumables</t>
+  </si>
+  <si>
+    <t>Production Charges</t>
+  </si>
+  <si>
+    <t>Replacement</t>
+  </si>
+  <si>
+    <t>Packaging</t>
+  </si>
+  <si>
+    <t>Booklet</t>
+  </si>
+  <si>
+    <t>Glycerine</t>
+  </si>
+  <si>
+    <t>Glycol</t>
+  </si>
+  <si>
+    <t>Flavour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicotine </t>
+  </si>
+  <si>
+    <t>Amber Bottle</t>
+  </si>
+  <si>
+    <t>Refill Bottle</t>
+  </si>
+  <si>
+    <t>Apple Madness</t>
+  </si>
+  <si>
+    <t>Razzle Dazzle</t>
+  </si>
+  <si>
+    <t>POLISH PACKS</t>
+  </si>
+  <si>
     <t>GEL NAIL LAMPS</t>
-  </si>
-  <si>
-    <t>PRODUCTION CHARGES</t>
-  </si>
-  <si>
-    <t>LIMITED EDITION</t>
-  </si>
-  <si>
-    <t>CHROME POWDER</t>
-  </si>
-  <si>
-    <t>GEL LAMP PACKS</t>
-  </si>
-  <si>
-    <t>Barcode</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Box</t>
-  </si>
-  <si>
-    <t>cin7_aged_trim</t>
-  </si>
-  <si>
-    <t>shipping</t>
-  </si>
-  <si>
-    <t>Street</t>
-  </si>
-  <si>
-    <t>Suburb</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Postcode</t>
-  </si>
-  <si>
-    <t>media_type</t>
-  </si>
-  <si>
-    <t>Packs</t>
-  </si>
-  <si>
-    <t>Consumables</t>
-  </si>
-  <si>
-    <t>Production Charges</t>
-  </si>
-  <si>
-    <t>Replacement</t>
-  </si>
-  <si>
-    <t>Packaging</t>
-  </si>
-  <si>
-    <t>Booklet</t>
-  </si>
-  <si>
-    <t>Glycerine</t>
-  </si>
-  <si>
-    <t>Glycol</t>
-  </si>
-  <si>
-    <t>Flavour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nicotine </t>
-  </si>
-  <si>
-    <t>Amber Bottle</t>
-  </si>
-  <si>
-    <t>Refill Bottle</t>
-  </si>
-  <si>
-    <t>Apple Madness</t>
-  </si>
-  <si>
-    <t>Razzle Dazzle</t>
   </si>
 </sst>
 </file>
@@ -1980,8 +1983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2357,16 +2360,16 @@
         <v>332</v>
       </c>
       <c r="J3" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>348</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>349</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>118</v>
@@ -2693,13 +2696,13 @@
         <v>316</v>
       </c>
       <c r="B6" t="s">
+        <v>338</v>
+      </c>
+      <c r="C6" t="s">
         <v>339</v>
       </c>
-      <c r="C6" t="s">
-        <v>336</v>
-      </c>
-      <c r="D6" t="s">
-        <v>340</v>
+      <c r="D6" s="2" t="s">
+        <v>365</v>
       </c>
       <c r="E6" t="s">
         <v>317</v>
@@ -2710,73 +2713,76 @@
       <c r="G6" t="s">
         <v>321</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>338</v>
+      <c r="H6" t="s">
+        <v>364</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>337</v>
+      <c r="L6" s="3" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C7" t="s">
         <v>341</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>342</v>
       </c>
-      <c r="D7" t="s">
-        <v>343</v>
-      </c>
       <c r="E7" t="s">
+        <v>350</v>
+      </c>
+      <c r="F7" t="s">
         <v>351</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>352</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>353</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>354</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>355</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" t="s">
         <v>357</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>358</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>359</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>360</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>361</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>362</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>363</v>
-      </c>
-      <c r="R7" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.3">
@@ -3052,7 +3058,7 @@
         <v>284</v>
       </c>
       <c r="I13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J13" t="s">
         <v>64</v>
@@ -3238,7 +3244,7 @@
         <v>322</v>
       </c>
       <c r="H16" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
post week 15 output cleanup - dates use nz timezone - downloading more robust - less duplication
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zander/Downloads/Automation-Gel 2/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61ED363B-2A0B-8148-9C6F-6B177C56B640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACF03A5-E9DD-48FF-B84E-27F1F5118028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="headers" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="370">
   <si>
     <t>shopify_orders</t>
   </si>
@@ -1073,12 +1073,6 @@
     <t>media_type</t>
   </si>
   <si>
-    <t>Packs</t>
-  </si>
-  <si>
-    <t>Consumables</t>
-  </si>
-  <si>
     <t>Production Charges</t>
   </si>
   <si>
@@ -1124,7 +1118,19 @@
     <t>production</t>
   </si>
   <si>
-    <t>consumables</t>
+    <t>cin7_fiter_names</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Pack</t>
+  </si>
+  <si>
+    <t>Consumable</t>
+  </si>
+  <si>
+    <t>consumable</t>
   </si>
 </sst>
 </file>
@@ -1623,7 +1629,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
@@ -1634,6 +1640,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1989,77 +1996,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ21"/>
+  <dimension ref="A1:BJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="50" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="41" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="65.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="47.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="65.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="47.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="34.44140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="36" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="41.33203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="37.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="36.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="39.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.77734375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="30" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="28" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="37.109375" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="40" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="61.83203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="61.77734375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="39.77734375" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="41.83203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="45.1640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="36.1640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="41.77734375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="38.77734375" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="43" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="20" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="27.77734375" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="22.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2151,7 +2158,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -2339,7 +2346,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>324</v>
       </c>
@@ -2383,7 +2390,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
@@ -2565,7 +2572,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>39</v>
       </c>
@@ -2699,7 +2706,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>316</v>
       </c>
@@ -2710,7 +2717,7 @@
         <v>339</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E6" t="s">
         <v>317</v>
@@ -2722,7 +2729,7 @@
         <v>321</v>
       </c>
       <c r="H6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>337</v>
@@ -2737,189 +2744,156 @@
         <v>336</v>
       </c>
     </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="B7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C7" t="s">
+        <v>368</v>
+      </c>
+      <c r="D7" t="s">
+        <v>340</v>
+      </c>
+      <c r="E7" t="s">
+        <v>367</v>
+      </c>
+      <c r="F7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="8" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>340</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>341</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>342</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
+        <v>367</v>
+      </c>
+      <c r="F8" t="s">
+        <v>368</v>
+      </c>
+      <c r="G8" t="s">
         <v>350</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H8" t="s">
         <v>351</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I8" t="s">
         <v>352</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J8" t="s">
         <v>353</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K8" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L8" t="s">
         <v>355</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="M8" t="s">
         <v>356</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N8" t="s">
         <v>357</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O8" t="s">
         <v>358</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P8" t="s">
         <v>359</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q8" t="s">
         <v>360</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R8" t="s">
         <v>361</v>
       </c>
-      <c r="Q7" t="s">
-        <v>362</v>
-      </c>
-      <c r="R7" t="s">
-        <v>363</v>
-      </c>
-      <c r="S7" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>367</v>
+      <c r="S8" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>369</v>
       </c>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>52</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>53</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>54</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>55</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" t="s">
         <v>56</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I9" t="s">
         <v>57</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J9" t="s">
         <v>58</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K9" t="s">
         <v>59</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L9" t="s">
         <v>60</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M9" t="s">
         <v>270</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N9" t="s">
         <v>271</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O9" t="s">
         <v>272</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P9" t="s">
         <v>273</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q9" t="s">
         <v>274</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R9" t="s">
         <v>275</v>
       </c>
-      <c r="S8" t="s">
+      <c r="S9" t="s">
         <v>276</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T9" t="s">
         <v>277</v>
       </c>
-      <c r="U8" t="s">
+      <c r="U9" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>297</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="D9" t="s">
-        <v>311</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="G9" t="s">
-        <v>310</v>
-      </c>
-      <c r="H9" t="s">
-        <v>298</v>
-      </c>
-      <c r="I9" t="s">
-        <v>299</v>
-      </c>
-      <c r="J9" t="s">
-        <v>300</v>
-      </c>
-      <c r="K9" t="s">
-        <v>301</v>
-      </c>
-      <c r="L9" t="s">
-        <v>302</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="N9" t="s">
-        <v>304</v>
-      </c>
-      <c r="O9" t="s">
-        <v>305</v>
-      </c>
-      <c r="P9" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>62</v>
@@ -2928,347 +2902,400 @@
         <v>279</v>
       </c>
       <c r="D10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="G10" t="s">
+        <v>310</v>
+      </c>
+      <c r="H10" t="s">
+        <v>298</v>
+      </c>
+      <c r="I10" t="s">
+        <v>299</v>
+      </c>
+      <c r="J10" t="s">
+        <v>300</v>
+      </c>
+      <c r="K10" t="s">
+        <v>301</v>
+      </c>
+      <c r="L10" t="s">
+        <v>302</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="N10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O10" t="s">
+        <v>305</v>
+      </c>
+      <c r="P10" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="11" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D11" t="s">
         <v>63</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>64</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>65</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>66</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>67</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I11" t="s">
         <v>68</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J11" t="s">
         <v>69</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K11" t="s">
         <v>70</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L11" t="s">
         <v>71</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>56</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>57</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>58</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>75</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>76</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>77</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>78</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>79</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>81</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I13" t="s">
         <v>82</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J13" t="s">
         <v>83</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K13" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L13" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="M13" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="N13" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="O13" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="P13" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="Q12" s="3" t="s">
+      <c r="Q13" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="R12" s="3" t="s">
+      <c r="R13" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="S12" s="3" t="s">
+      <c r="S13" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="T12" s="3" t="s">
+      <c r="T13" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="U12" s="3" t="s">
+      <c r="U13" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="V12" s="3" t="s">
+      <c r="V13" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="W12" s="3" t="s">
+      <c r="W13" s="3" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>86</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>282</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>283</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>76</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H14" t="s">
         <v>284</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I14" t="s">
         <v>349</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>88</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>89</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>90</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>91</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>92</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>93</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H15" t="s">
         <v>94</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I15" t="s">
         <v>95</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J15" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="K15" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="L15" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M15" t="s">
         <v>99</v>
       </c>
-      <c r="N14" s="3" t="s">
+      <c r="N15" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O15" t="s">
         <v>101</v>
       </c>
-      <c r="P14" s="3" t="s">
+      <c r="P15" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="Q15" t="s">
         <v>103</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R15" t="s">
         <v>104</v>
       </c>
-      <c r="S14" t="s">
+      <c r="S15" t="s">
         <v>105</v>
       </c>
-      <c r="T14" s="3" t="s">
+      <c r="T15" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="U14" t="s">
+      <c r="U15" t="s">
         <v>107</v>
       </c>
-      <c r="V14" s="3" t="s">
+      <c r="V15" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="W14" s="3" t="s">
+      <c r="W15" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="X14" t="s">
+      <c r="X15" t="s">
         <v>110</v>
       </c>
-      <c r="Y14" s="3" t="s">
+      <c r="Y15" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="Z14" s="3" t="s">
+      <c r="Z15" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="AA14" s="3" t="s">
+      <c r="AA15" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="AB14" s="3" t="s">
+      <c r="AB15" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="AC14" s="3" t="s">
+      <c r="AC15" s="3" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>116</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" t="s">
         <v>117</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
         <v>118</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H16" t="s">
         <v>119</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K16" t="s">
         <v>122</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L16" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="N16" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="O16" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="P16" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="Q16" t="s">
         <v>128</v>
       </c>
-      <c r="R15" t="s">
+      <c r="R16" t="s">
         <v>129</v>
       </c>
-      <c r="S15" t="s">
+      <c r="S16" t="s">
         <v>130</v>
       </c>
-      <c r="T15" t="s">
+      <c r="T16" t="s">
         <v>131</v>
       </c>
-      <c r="U15" t="s">
+      <c r="U16" t="s">
         <v>132</v>
       </c>
-      <c r="V15" t="s">
+      <c r="V16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>312</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>313</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>2792653102</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>315</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>323</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
         <v>322</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H17" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3286,9 +3313,9 @@
       <selection activeCell="C1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>134</v>
       </c>

</xml_diff>

<commit_message>
download further robustness changes date fix for product instagram pics 'engagement' removed
</commit_message>
<xml_diff>
--- a/config/headers.xlsx
+++ b/config/headers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zander\IdeaProjects\Automation-Gel\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACF03A5-E9DD-48FF-B84E-27F1F5118028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C724ABD6-122A-4C8F-9FEB-A59F516BC216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="headers" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="371">
   <si>
     <t>shopify_orders</t>
   </si>
@@ -1131,6 +1131,9 @@
   </si>
   <si>
     <t>consumable</t>
+  </si>
+  <si>
+    <t>Product Name</t>
   </si>
 </sst>
 </file>
@@ -1999,7 +2002,7 @@
   <dimension ref="A1:BJ22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2389,6 +2392,9 @@
       <c r="N3" s="5" t="s">
         <v>118</v>
       </c>
+      <c r="O3" s="5" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">

</xml_diff>